<commit_message>
Point TextMarkerText DB and Content Editor Support
</commit_message>
<xml_diff>
--- a/PointlessWaymarks.CmsTests/TestMedia/GrandCanyonPointsImport.xlsx
+++ b/PointlessWaymarks.CmsTests/TestMedia/GrandCanyonPointsImport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PointlessWaymarksCms05\PointlessWaymarksTests\IronwoodTestContent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PointlessWaymarksCms03\PointlessWaymarks.CmsTests\TestMedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B81FD2-E5B3-415A-9570-B12E13A8FDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7697D7-3BFB-4F5B-853D-60629C01BB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="25600" windowHeight="13760" xr2:uid="{A502E4A2-19B3-43B1-97B2-6120C4E9A4F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{A502E4A2-19B3-43B1-97B2-6120C4E9A4F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="381">
   <si>
     <t>MarkdigMarkdown01</t>
   </si>
@@ -1144,6 +1144,42 @@
   </si>
   <si>
     <t>PointDetail 1</t>
+  </si>
+  <si>
+    <t>TextMarkerText</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -1211,15 +1247,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="39">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1281,6 +1309,15 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1309,6 +1346,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1613,42 +1658,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1208738D-823F-465D-AA3D-EB5F2F01FEA0}" name="Table1" displayName="Table1" ref="A1:AK99" totalsRowShown="0" dataDxfId="37">
-  <tableColumns count="37">
-    <tableColumn id="1" xr3:uid="{D2E58667-7262-4F8A-8CBB-4AF358AB7A7C}" name="FEATURE_ID" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{11E65206-D51B-40D1-957D-D316CAFD2787}" name="FEATURE_NAME" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{FDF47325-247C-43BF-895C-E73292CC8D78}" name="FEATURE_CLASS" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{9D62ADD6-2337-4335-BA17-604B3979C5A7}" name="STATE_ALPHA" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{C6D1D603-2797-4243-BF10-DAB2B81CCE1D}" name="STATE_NUMERIC" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{7D0D4BE9-0AB1-48CE-99DD-AE04EFA9AA79}" name="COUNTY_NAME" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{E8C29E4E-09E0-45E2-8463-ED9C0E8C2449}" name="COUNTY_NUMERIC" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{4828066A-6EF8-4EBC-85CD-BE4F87BEAD4A}" name="PRIMARY_LAT_DMS" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{E0509827-3112-48B6-973A-8D777F1EE359}" name="PRIM_LONG_DMS" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{D80AA723-8937-42AC-B3C9-E07111556009}" name="PRIM_LAT_DEC" dataDxfId="27"/>
-    <tableColumn id="11" xr3:uid="{BD57E42C-4DE9-4BBB-A7AB-4DFFD619076A}" name="PRIM_LONG_DEC" dataDxfId="26"/>
-    <tableColumn id="12" xr3:uid="{D7898E1C-2DCB-40E7-AD40-FA121B021698}" name="SOURCE_LAT_DMS" dataDxfId="25"/>
-    <tableColumn id="13" xr3:uid="{E564D70C-DFE5-4CDC-A855-7CAFCD54BA99}" name="SOURCE_LONG_DMS" dataDxfId="24"/>
-    <tableColumn id="14" xr3:uid="{96E90ABF-38F0-4D4E-A783-4601C2F9FA62}" name="SOURCE_LAT_DEC" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{C87BF9FC-F238-4CA8-AFF8-91541EC9C60D}" name="SOURCE_LONG_DEC" dataDxfId="22"/>
-    <tableColumn id="16" xr3:uid="{153857A4-41D9-4FCD-A0A7-45712CD94DDA}" name="ELEV_IN_M" dataDxfId="21"/>
-    <tableColumn id="17" xr3:uid="{9D62C92A-0DA1-44EC-AFA5-66BB6C44A975}" name="ELEV_IN_FT" dataDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{D6A168FE-46ED-4827-8721-43B917D8857C}" name="MAP_NAME" dataDxfId="19"/>
-    <tableColumn id="19" xr3:uid="{1D8AB82A-6631-4B9D-99A8-A5E406A95200}" name="DATE_CREATED" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{4D75BFFB-B2B9-4C59-B8DD-08ED5DCF56D3}" name="DATE_EDITED" dataDxfId="17"/>
-    <tableColumn id="21" xr3:uid="{D776A8A8-1088-4B22-92E7-A967C7ACA1E6}" name="NewContentType" dataDxfId="16"/>
-    <tableColumn id="22" xr3:uid="{BCBF2563-27DE-4A45-9009-7517692DA782}" name="Title" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1208738D-823F-465D-AA3D-EB5F2F01FEA0}" name="Table1" displayName="Table1" ref="A1:AL99" totalsRowShown="0" dataDxfId="38">
+  <tableColumns count="38">
+    <tableColumn id="1" xr3:uid="{D2E58667-7262-4F8A-8CBB-4AF358AB7A7C}" name="FEATURE_ID" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{11E65206-D51B-40D1-957D-D316CAFD2787}" name="FEATURE_NAME" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{FDF47325-247C-43BF-895C-E73292CC8D78}" name="FEATURE_CLASS" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{9D62ADD6-2337-4335-BA17-604B3979C5A7}" name="STATE_ALPHA" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{C6D1D603-2797-4243-BF10-DAB2B81CCE1D}" name="STATE_NUMERIC" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{7D0D4BE9-0AB1-48CE-99DD-AE04EFA9AA79}" name="COUNTY_NAME" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{E8C29E4E-09E0-45E2-8463-ED9C0E8C2449}" name="COUNTY_NUMERIC" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{4828066A-6EF8-4EBC-85CD-BE4F87BEAD4A}" name="PRIMARY_LAT_DMS" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{E0509827-3112-48B6-973A-8D777F1EE359}" name="PRIM_LONG_DMS" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{D80AA723-8937-42AC-B3C9-E07111556009}" name="PRIM_LAT_DEC" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{BD57E42C-4DE9-4BBB-A7AB-4DFFD619076A}" name="PRIM_LONG_DEC" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{D7898E1C-2DCB-40E7-AD40-FA121B021698}" name="SOURCE_LAT_DMS" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{E564D70C-DFE5-4CDC-A855-7CAFCD54BA99}" name="SOURCE_LONG_DMS" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{96E90ABF-38F0-4D4E-A783-4601C2F9FA62}" name="SOURCE_LAT_DEC" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{C87BF9FC-F238-4CA8-AFF8-91541EC9C60D}" name="SOURCE_LONG_DEC" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{153857A4-41D9-4FCD-A0A7-45712CD94DDA}" name="ELEV_IN_M" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{9D62C92A-0DA1-44EC-AFA5-66BB6C44A975}" name="ELEV_IN_FT" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{D6A168FE-46ED-4827-8721-43B917D8857C}" name="MAP_NAME" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{1D8AB82A-6631-4B9D-99A8-A5E406A95200}" name="DATE_CREATED" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{4D75BFFB-B2B9-4C59-B8DD-08ED5DCF56D3}" name="DATE_EDITED" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{D776A8A8-1088-4B22-92E7-A967C7ACA1E6}" name="NewContentType" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{BCBF2563-27DE-4A45-9009-7517692DA782}" name="Title" dataDxfId="16">
       <calculatedColumnFormula>B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{1B009923-0625-4FAC-B7F5-DCE848005123}" name="Slug" dataDxfId="14">
+    <tableColumn id="23" xr3:uid="{1B009923-0625-4FAC-B7F5-DCE848005123}" name="Slug" dataDxfId="15">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(V2), " ", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{45265D90-DD2D-4207-B91D-9163A9B19D74}" name="BodyContent" dataDxfId="13"/>
-    <tableColumn id="25" xr3:uid="{80C4B639-0A9E-4D97-B29E-A7F8DDA9B0B3}" name="BodyContentFormat" dataDxfId="12"/>
-    <tableColumn id="26" xr3:uid="{85E3548B-666A-4B25-B156-AFF5123DE955}" name="UpdateNotesFormat" dataDxfId="11"/>
-    <tableColumn id="27" xr3:uid="{E609B391-60DB-4FD0-BA56-92ECCFD26CDC}" name="Latitude" dataDxfId="10">
+    <tableColumn id="24" xr3:uid="{45265D90-DD2D-4207-B91D-9163A9B19D74}" name="BodyContent" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{80C4B639-0A9E-4D97-B29E-A7F8DDA9B0B3}" name="BodyContentFormat" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{85E3548B-666A-4B25-B156-AFF5123DE955}" name="UpdateNotesFormat" dataDxfId="12"/>
+    <tableColumn id="27" xr3:uid="{E609B391-60DB-4FD0-BA56-92ECCFD26CDC}" name="Latitude" dataDxfId="11">
       <calculatedColumnFormula>J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{3EB02439-D402-4820-A58D-32055C4FB187}" name="Longitude" dataDxfId="0">
+    <tableColumn id="28" xr3:uid="{3EB02439-D402-4820-A58D-32055C4FB187}" name="Longitude" dataDxfId="10">
       <calculatedColumnFormula>K2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="29" xr3:uid="{57726F3C-3D0A-4F88-8A54-44F1D05E6C01}" name="Elevation" dataDxfId="9">
@@ -1662,10 +1707,11 @@
     <tableColumn id="33" xr3:uid="{83B88F62-B46F-4CED-A530-3B101E8CBBFA}" name="Tags" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.CONCAT("grand canyon, ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{6B0E8F35-25DB-4BD6-93F3-2E2E8DBACA78}" name="CreatedBy" dataDxfId="4"/>
-    <tableColumn id="35" xr3:uid="{2CCAFA83-E69E-4E91-92D8-DF4C6DC8F9FC}" name="CreatedOn" dataDxfId="3"/>
-    <tableColumn id="36" xr3:uid="{DEE1C7CE-9A12-46E0-B3F8-8B00D65FFA10}" name="UpdateContentFormat" dataDxfId="2"/>
-    <tableColumn id="37" xr3:uid="{83A7D6D9-9F51-4C21-A2CB-179160B8B0D4}" name="PointDetail 1" dataDxfId="1">
+    <tableColumn id="38" xr3:uid="{8ECFFA9E-BE30-4C9B-81AD-E8FBE61FCB97}" name="TextMarkerText" dataDxfId="4"/>
+    <tableColumn id="34" xr3:uid="{6B0E8F35-25DB-4BD6-93F3-2E2E8DBACA78}" name="CreatedBy" dataDxfId="3"/>
+    <tableColumn id="35" xr3:uid="{2CCAFA83-E69E-4E91-92D8-DF4C6DC8F9FC}" name="CreatedOn" dataDxfId="2"/>
+    <tableColumn id="36" xr3:uid="{DEE1C7CE-9A12-46E0-B3F8-8B00D65FFA10}" name="UpdateContentFormat" dataDxfId="1"/>
+    <tableColumn id="37" xr3:uid="{83A7D6D9-9F51-4C21-A2CB-179160B8B0D4}" name="PointDetail 1" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT("ContentId:||Type:Feature||Data:{""DataTypeIdentifier"":""Feature"",""Type"":""",C2,""",""Notes"":""GNIS Feature ID:",A2,", ", F2," County, ",D2,". USGS 7.5' Quad: ",R2,". GNIS Elevation: ", Q2,"'. GNIS Entry Created: ", TEXT(S2,"M/D/YYYY"),IF(ISBLANK(T2),".",_xlfn.CONCAT(", Updated: ", TEXT(T2,"M/D/YYYY"),". ")),"""}")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1970,52 +2016,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5FEDEF-5A8E-421A-8857-D6C400357593}">
-  <dimension ref="A1:AK99"/>
+  <dimension ref="A1:AL99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="X40" workbookViewId="0">
+      <selection activeCell="AH43" sqref="AH43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" customWidth="1"/>
-    <col min="9" max="9" width="17.90625" customWidth="1"/>
-    <col min="10" max="10" width="15.6328125" customWidth="1"/>
-    <col min="11" max="11" width="17.36328125" customWidth="1"/>
-    <col min="12" max="12" width="18.453125" customWidth="1"/>
-    <col min="13" max="13" width="20.1796875" customWidth="1"/>
-    <col min="14" max="14" width="17.90625" customWidth="1"/>
-    <col min="15" max="15" width="19.6328125" customWidth="1"/>
-    <col min="16" max="16" width="12.36328125" customWidth="1"/>
-    <col min="17" max="17" width="12.54296875" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="15.90625" customWidth="1"/>
-    <col min="20" max="20" width="14.36328125" customWidth="1"/>
-    <col min="21" max="21" width="17.36328125" customWidth="1"/>
-    <col min="22" max="22" width="66.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="65.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.81640625" customWidth="1"/>
-    <col min="25" max="25" width="19.90625" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" customWidth="1"/>
+    <col min="22" max="22" width="66.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" customWidth="1"/>
+    <col min="25" max="25" width="19.85546875" customWidth="1"/>
     <col min="26" max="26" width="20" customWidth="1"/>
-    <col min="27" max="27" width="9.7265625" customWidth="1"/>
-    <col min="28" max="28" width="11.08984375" customWidth="1"/>
-    <col min="29" max="29" width="10.54296875" customWidth="1"/>
-    <col min="31" max="31" width="20.36328125" customWidth="1"/>
-    <col min="32" max="32" width="10.7265625" customWidth="1"/>
-    <col min="34" max="34" width="11.453125" customWidth="1"/>
-    <col min="35" max="35" width="11.90625" customWidth="1"/>
-    <col min="36" max="36" width="21.90625" customWidth="1"/>
-    <col min="37" max="37" width="73.7265625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" customWidth="1"/>
+    <col min="31" max="31" width="20.42578125" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="11.42578125" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" customWidth="1"/>
+    <col min="37" max="37" width="21.85546875" customWidth="1"/>
+    <col min="38" max="38" width="73.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>359</v>
       </c>
@@ -2116,19 +2162,22 @@
         <v>329</v>
       </c>
       <c r="AH1" t="s">
+        <v>369</v>
+      </c>
+      <c r="AI1" t="s">
         <v>364</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>363</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>328</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1058</v>
       </c>
@@ -2226,20 +2275,23 @@
         <v>grand canyon, Bass Tank</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AJ2" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="5" t="str">
-        <f t="shared" ref="AK2:AK65" si="7">_xlfn.CONCAT("ContentId:||Type:Feature||Data:{""DataTypeIdentifier"":""Feature"",""Type"":""",C2,""",""Notes"":""GNIS Feature ID:",A2,", ", F2," County, ",D2,". USGS 7.5' Quad: ",R2,". GNIS Elevation: ", Q2,"'. GNIS Entry Created: ", TEXT(S2,"M/D/YYYY"),IF(ISBLANK(T2),".",_xlfn.CONCAT(", Updated: ", TEXT(T2,"M/D/YYYY"),". ")),"""}")</f>
+      <c r="AK2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="5" t="str">
+        <f t="shared" ref="AL2:AL65" si="7">_xlfn.CONCAT("ContentId:||Type:Feature||Data:{""DataTypeIdentifier"":""Feature"",""Type"":""",C2,""",""Notes"":""GNIS Feature ID:",A2,", ", F2," County, ",D2,". USGS 7.5' Quad: ",R2,". GNIS Elevation: ", Q2,"'. GNIS Entry Created: ", TEXT(S2,"M/D/YYYY"),IF(ISBLANK(T2),".",_xlfn.CONCAT(", Updated: ", TEXT(T2,"M/D/YYYY"),". ")),"""}")</f>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:1058, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6253'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1860</v>
       </c>
@@ -2343,20 +2395,23 @@
         <v>grand canyon, Boucher Creek</v>
       </c>
       <c r="AH3" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI3" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AJ3" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="5" t="str">
+      <c r="AK3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:1860, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2356'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1861</v>
       </c>
@@ -2454,20 +2509,23 @@
         <v>grand canyon, Boucher Rapids</v>
       </c>
       <c r="AH4" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI4" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AJ4" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="5" t="str">
+      <c r="AK4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Rapids","Notes":"GNIS Feature ID:1861, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2333'. GNIS Entry Created: 2/8/1980, Updated: 6/7/2011. "}</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1948</v>
       </c>
@@ -2563,20 +2621,23 @@
         <v>grand canyon, Breezy Point</v>
       </c>
       <c r="AH5" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI5" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="AJ5" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="5" t="str">
+      <c r="AK5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:1948, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4416'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1965</v>
       </c>
@@ -2674,20 +2735,23 @@
         <v>grand canyon, Bright Angel Trail</v>
       </c>
       <c r="AH6" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI6" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AJ6" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="5" t="str">
+      <c r="AK6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Trail","Notes":"GNIS Feature ID:1965, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4124'. GNIS Entry Created: 2/8/1980, Updated: 3/22/2011. "}</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1966</v>
       </c>
@@ -2791,20 +2855,23 @@
         <v>grand canyon, Bright Angel Wash</v>
       </c>
       <c r="AH7" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI7" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI7" s="3">
+      <c r="AJ7" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="5" t="str">
+      <c r="AK7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:1966, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6273'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2026</v>
       </c>
@@ -2902,20 +2969,23 @@
         <v>grand canyon, Brush Tank</v>
       </c>
       <c r="AH8" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI8" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI8" s="3">
+      <c r="AJ8" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="5" t="str">
+      <c r="AK8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:2026, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6237'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2571</v>
       </c>
@@ -3011,20 +3081,23 @@
         <v>grand canyon, Cathedral Stairs</v>
       </c>
       <c r="AH9" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="AI9" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI9" s="3">
+      <c r="AJ9" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="5" t="str">
+      <c r="AK9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:2571, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4462'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2654</v>
       </c>
@@ -3122,20 +3195,23 @@
         <v>grand canyon, Cedar Spring</v>
       </c>
       <c r="AH10" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="AI10" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI10" s="3">
+      <c r="AJ10" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="5" t="str">
+      <c r="AK10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Spring","Notes":"GNIS Feature ID:2654, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 3343'. GNIS Entry Created: 2/8/1980, Updated: 4/18/2011. "}</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3087</v>
       </c>
@@ -3231,20 +3307,23 @@
         <v>grand canyon, Cocopa Point</v>
       </c>
       <c r="AH11" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="AI11" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI11" s="3">
+      <c r="AJ11" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="5" t="str">
+      <c r="AK11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:3087, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6627'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3138</v>
       </c>
@@ -3340,20 +3419,23 @@
         <v>grand canyon, Columbus Point</v>
       </c>
       <c r="AH12" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="AI12" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI12" s="3">
+      <c r="AJ12" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="5" t="str">
+      <c r="AK12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:3138, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4514'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3208</v>
       </c>
@@ -3451,20 +3533,23 @@
         <v>grand canyon, Cope Butte</v>
       </c>
       <c r="AH13" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="AI13" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI13" s="3">
+      <c r="AJ13" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="5" t="str">
+      <c r="AK13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:3208, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4518'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>3686</v>
       </c>
@@ -3562,20 +3647,23 @@
         <v>grand canyon, Dana Butte</v>
       </c>
       <c r="AH14" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="AI14" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI14" s="3">
+      <c r="AJ14" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="5" t="str">
+      <c r="AK14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:3686, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5010'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>3935</v>
       </c>
@@ -3673,20 +3761,23 @@
         <v>grand canyon, Diana Temple</v>
       </c>
       <c r="AH15" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="AI15" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI15" s="3">
+      <c r="AJ15" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="5" t="str">
+      <c r="AK15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:3935, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6673'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4113</v>
       </c>
@@ -3784,20 +3875,23 @@
         <v>grand canyon, Dripping Spring</v>
       </c>
       <c r="AH16" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="AI16" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI16" s="3">
+      <c r="AJ16" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK16" s="5" t="str">
+      <c r="AK16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Spring","Notes":"GNIS Feature ID:4113, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5440'. GNIS Entry Created: 2/8/1980, Updated: 4/18/2011. "}</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4122</v>
       </c>
@@ -3893,20 +3987,23 @@
         <v>grand canyon, Dripping Springs Trail</v>
       </c>
       <c r="AH17" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="AI17" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI17" s="3">
+      <c r="AJ17" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK17" s="5" t="str">
+      <c r="AK17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Trail","Notes":"GNIS Feature ID:4122, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5358'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>4465</v>
       </c>
@@ -4004,20 +4101,23 @@
         <v>grand canyon, Eremita Mesa</v>
       </c>
       <c r="AH18" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="AI18" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI18" s="3">
+      <c r="AJ18" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK18" s="5" t="str">
+      <c r="AK18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:4465, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6617'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>4466</v>
       </c>
@@ -4115,20 +4215,23 @@
         <v>grand canyon, Eremita Tank</v>
       </c>
       <c r="AH19" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="AI19" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI19" s="3">
+      <c r="AJ19" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK19" s="5" t="str">
+      <c r="AK19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:4466, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6365'. GNIS Entry Created: 2/8/1980, Updated: 3/15/2019. "}</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>4791</v>
       </c>
@@ -4224,20 +4327,23 @@
         <v>grand canyon, Fourmile Spring</v>
       </c>
       <c r="AH20" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="AI20" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI20" s="3">
+      <c r="AJ20" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK20" s="5" t="str">
+      <c r="AK20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Spring","Notes":"GNIS Feature ID:4791, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4373'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>5213</v>
       </c>
@@ -4335,20 +4441,23 @@
         <v>grand canyon, Grand Canyon</v>
       </c>
       <c r="AH21" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AI21" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI21" s="3">
+      <c r="AJ21" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK21" s="5" t="str">
+      <c r="AK21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Populated Place","Notes":"GNIS Feature ID:5213, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6886'. GNIS Entry Created: 6/27/1984, Updated: 9/23/2008. "}</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>5254</v>
       </c>
@@ -4446,20 +4555,23 @@
         <v>grand canyon, Granite Rapids</v>
       </c>
       <c r="AH22" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AI22" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI22" s="3">
+      <c r="AJ22" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK22" s="5" t="str">
+      <c r="AK22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Rapids","Notes":"GNIS Feature ID:5254, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2359'. GNIS Entry Created: 2/8/1980, Updated: 3/15/2019. "}</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>5344</v>
       </c>
@@ -4555,20 +4667,23 @@
         <v>grand canyon, Great Mohave Wall</v>
       </c>
       <c r="AH23" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AI23" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI23" s="3">
+      <c r="AJ23" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK23" s="5" t="str">
+      <c r="AK23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:5344, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6496'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>5736</v>
       </c>
@@ -4672,20 +4787,23 @@
         <v>grand canyon, Hermit Creek</v>
       </c>
       <c r="AH24" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI24" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI24" s="3">
+      <c r="AJ24" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK24" s="5" t="str">
+      <c r="AK24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:5736, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2365'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>5737</v>
       </c>
@@ -4783,20 +4901,23 @@
         <v>grand canyon, Hermit Rapids</v>
       </c>
       <c r="AH25" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI25" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI25" s="3">
+      <c r="AJ25" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ25" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK25" s="5" t="str">
+      <c r="AK25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Rapids","Notes":"GNIS Feature ID:5737, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2342'. GNIS Entry Created: 2/8/1980, Updated: 3/15/2019. "}</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>5738</v>
       </c>
@@ -4892,20 +5013,23 @@
         <v>grand canyon, Hermit Trail</v>
       </c>
       <c r="AH26" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI26" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI26" s="3">
+      <c r="AJ26" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK26" s="5" t="str">
+      <c r="AK26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Trail","Notes":"GNIS Feature ID:5738, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4928'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>5740</v>
       </c>
@@ -5001,20 +5125,23 @@
         <v>grand canyon, Hermits Rest</v>
       </c>
       <c r="AH27" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI27" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI27" s="3">
+      <c r="AJ27" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ27" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK27" s="5" t="str">
+      <c r="AK27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Locale","Notes":"GNIS Feature ID:5740, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6660'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>5905</v>
       </c>
@@ -5112,20 +5239,23 @@
         <v>grand canyon, Homestead Tank</v>
       </c>
       <c r="AH28" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI28" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI28" s="3">
+      <c r="AJ28" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK28" s="5" t="str">
+      <c r="AK28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:5905, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6237'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>5933</v>
       </c>
@@ -5221,20 +5351,23 @@
         <v>grand canyon, Hopi Point</v>
       </c>
       <c r="AH29" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI29" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI29" s="3">
+      <c r="AJ29" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK29" s="5" t="str">
+      <c r="AK29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:5933, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6401'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>5935</v>
       </c>
@@ -5332,20 +5465,23 @@
         <v>grand canyon, Hopi Wall</v>
       </c>
       <c r="AH30" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI30" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI30" s="3">
+      <c r="AJ30" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ30" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK30" s="5" t="str">
+      <c r="AK30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:5935, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6909'. GNIS Entry Created: 2/8/1980, Updated: 3/22/2011. "}</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>5937</v>
       </c>
@@ -5449,20 +5585,23 @@
         <v>grand canyon, Horn Creek</v>
       </c>
       <c r="AH31" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI31" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI31" s="3">
+      <c r="AJ31" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK31" s="5" t="str">
+      <c r="AK31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:5937, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2825'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>5938</v>
       </c>
@@ -5560,20 +5699,23 @@
         <v>grand canyon, Horn Creek Rapids</v>
       </c>
       <c r="AH32" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI32" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI32" s="3">
+      <c r="AJ32" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ32" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK32" s="5" t="str">
+      <c r="AK32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Rapids","Notes":"GNIS Feature ID:5938, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2388'. GNIS Entry Created: 2/8/1980, Updated: 3/15/2019. "}</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>6022</v>
       </c>
@@ -5671,20 +5813,23 @@
         <v>grand canyon, Horsethief Tank</v>
       </c>
       <c r="AH33" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI33" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI33" s="3">
+      <c r="AJ33" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ33" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK33" s="5" t="str">
+      <c r="AK33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:6022, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6384'. GNIS Entry Created: 2/8/1980, Updated: 3/15/2019. "}</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>6178</v>
       </c>
@@ -5782,20 +5927,23 @@
         <v>grand canyon, Ike Smith Tank</v>
       </c>
       <c r="AH34" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="AI34" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI34" s="3">
+      <c r="AJ34" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ34" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK34" s="5" t="str">
+      <c r="AK34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:6178, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6207'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>6411</v>
       </c>
@@ -5891,20 +6039,23 @@
         <v>grand canyon, Jicarilla Point</v>
       </c>
       <c r="AH35" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="AI35" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI35" s="3">
+      <c r="AJ35" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ35" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK35" s="5" t="str">
+      <c r="AK35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:6411, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6565'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>7163</v>
       </c>
@@ -6002,20 +6153,23 @@
         <v>grand canyon, Little Rain Tank</v>
       </c>
       <c r="AH36" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="AI36" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI36" s="3">
+      <c r="AJ36" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ36" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK36" s="5" t="str">
+      <c r="AK36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:7163, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6171'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>7367</v>
       </c>
@@ -6111,20 +6265,23 @@
         <v>grand canyon, Lookout Point</v>
       </c>
       <c r="AH37" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="AI37" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI37" s="3">
+      <c r="AJ37" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ37" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK37" s="5" t="str">
+      <c r="AK37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:7367, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4541'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>7700</v>
       </c>
@@ -6220,20 +6377,23 @@
         <v>grand canyon, Maricopa Point</v>
       </c>
       <c r="AH38" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI38" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI38" s="3">
+      <c r="AJ38" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK38" s="5" t="str">
+      <c r="AK38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:7700, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6854'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>7724</v>
       </c>
@@ -6331,20 +6491,23 @@
         <v>grand canyon, Marsh Butte</v>
       </c>
       <c r="AH39" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI39" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI39" s="3">
+      <c r="AJ39" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK39" s="5" t="str">
+      <c r="AK39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:7724, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4718'. GNIS Entry Created: 6/27/1984, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>7925</v>
       </c>
@@ -6440,20 +6603,23 @@
         <v>grand canyon, Mescalero Point</v>
       </c>
       <c r="AH40" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI40" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI40" s="3">
+      <c r="AJ40" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK40" s="5" t="str">
+      <c r="AK40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:7925, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6627'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>8033</v>
       </c>
@@ -6551,20 +6717,23 @@
         <v>grand canyon, Midway Number One Tank</v>
       </c>
       <c r="AH41" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI41" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI41" s="3">
+      <c r="AJ41" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ41" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK41" s="5" t="str">
+      <c r="AK41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:8033, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6132'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>8034</v>
       </c>
@@ -6662,20 +6831,23 @@
         <v>grand canyon, Midway Number Two Tank</v>
       </c>
       <c r="AH42" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI42" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI42" s="3">
+      <c r="AJ42" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ42" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK42" s="5" t="str">
+      <c r="AK42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL42" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:8034, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6181'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>8085</v>
       </c>
@@ -6771,20 +6943,23 @@
         <v>grand canyon, Mimbreno Point</v>
       </c>
       <c r="AH43" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI43" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI43" s="3">
+      <c r="AJ43" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ43" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK43" s="5" t="str">
+      <c r="AK43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL43" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:8085, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6608'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>8168</v>
       </c>
@@ -6880,20 +7055,23 @@
         <v>grand canyon, Mohave Point</v>
       </c>
       <c r="AH44" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI44" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI44" s="3">
+      <c r="AJ44" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK44" s="5" t="str">
+      <c r="AK44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL44" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:8168, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6988'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>8237</v>
       </c>
@@ -6997,20 +7175,23 @@
         <v>grand canyon, Monument Creek</v>
       </c>
       <c r="AH45" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI45" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI45" s="3">
+      <c r="AJ45" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK45" s="5" t="str">
+      <c r="AK45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:8237, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2388'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>8620</v>
       </c>
@@ -7107,21 +7288,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, New Tank</v>
       </c>
-      <c r="AH46" s="2" t="s">
+      <c r="AH46" s="2"/>
+      <c r="AI46" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI46" s="3">
+      <c r="AJ46" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ46" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK46" s="5" t="str">
+      <c r="AK46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:8620, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6076'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>8665</v>
       </c>
@@ -7224,21 +7406,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Ninetyfour Mile Creek</v>
       </c>
-      <c r="AH47" s="2" t="s">
+      <c r="AH47" s="2"/>
+      <c r="AI47" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI47" s="3">
+      <c r="AJ47" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK47" s="5" t="str">
+      <c r="AK47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:8665, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2349'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>8666</v>
       </c>
@@ -7341,21 +7524,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Ninetyone Mile Creek</v>
       </c>
-      <c r="AH48" s="2" t="s">
+      <c r="AH48" s="2"/>
+      <c r="AI48" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI48" s="3">
+      <c r="AJ48" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ48" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK48" s="5" t="str">
+      <c r="AK48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL48" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:8666, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2382'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>8842</v>
       </c>
@@ -7451,21 +7635,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, O'Connell Tank</v>
       </c>
-      <c r="AH49" s="2" t="s">
+      <c r="AH49" s="2"/>
+      <c r="AI49" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI49" s="3">
+      <c r="AJ49" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ49" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK49" s="5" t="str">
+      <c r="AK49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL49" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:8842, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6191'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>9442</v>
       </c>
@@ -7562,21 +7747,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Pima Point</v>
       </c>
-      <c r="AH50" s="2" t="s">
+      <c r="AH50" s="2"/>
+      <c r="AI50" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI50" s="3">
+      <c r="AJ50" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ50" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK50" s="5" t="str">
+      <c r="AK50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL50" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:9442, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6575'. GNIS Entry Created: 2/8/1980, Updated: 3/22/2011. "}</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>9556</v>
       </c>
@@ -7671,21 +7857,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Piute Point</v>
       </c>
-      <c r="AH51" s="2" t="s">
+      <c r="AH51" s="2"/>
+      <c r="AI51" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI51" s="3">
+      <c r="AJ51" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ51" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK51" s="5" t="str">
+      <c r="AK51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:9556, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6601'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>9627</v>
       </c>
@@ -7782,21 +7969,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Pollux Temple</v>
       </c>
-      <c r="AH52" s="2" t="s">
+      <c r="AH52" s="2"/>
+      <c r="AI52" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI52" s="3">
+      <c r="AJ52" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ52" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK52" s="5" t="str">
+      <c r="AK52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:9627, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6250'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>9721</v>
       </c>
@@ -7891,21 +8079,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Powell Point</v>
       </c>
-      <c r="AH53" s="2" t="s">
+      <c r="AH53" s="2"/>
+      <c r="AI53" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI53" s="3">
+      <c r="AJ53" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ53" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK53" s="5" t="str">
+      <c r="AK53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:9721, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5994'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>10564</v>
       </c>
@@ -8002,21 +8191,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Rowes Well</v>
       </c>
-      <c r="AH54" s="2" t="s">
+      <c r="AH54" s="2"/>
+      <c r="AI54" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI54" s="3">
+      <c r="AJ54" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ54" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK54" s="5" t="str">
+      <c r="AK54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL54" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Well","Notes":"GNIS Feature ID:10564, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6680'. GNIS Entry Created: 2/8/1980, Updated: 12/5/2017. "}</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>10746</v>
       </c>
@@ -8119,21 +8309,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Salt Creek</v>
       </c>
-      <c r="AH55" s="2" t="s">
+      <c r="AH55" s="2"/>
+      <c r="AI55" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI55" s="3">
+      <c r="AJ55" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ55" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK55" s="5" t="str">
+      <c r="AK55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL55" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:10746, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2487'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>10750</v>
       </c>
@@ -8230,21 +8421,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Salt Creek Rapids</v>
       </c>
-      <c r="AH56" s="2" t="s">
+      <c r="AH56" s="2"/>
+      <c r="AI56" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI56" s="3">
+      <c r="AJ56" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ56" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK56" s="5" t="str">
+      <c r="AK56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Rapids","Notes":"GNIS Feature ID:10750, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2369'. GNIS Entry Created: 2/8/1980, Updated: 3/15/2019. "}</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>10796</v>
       </c>
@@ -8341,21 +8533,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Sam Moore Tank</v>
       </c>
-      <c r="AH57" s="2" t="s">
+      <c r="AH57" s="2"/>
+      <c r="AI57" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI57" s="3">
+      <c r="AJ57" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ57" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK57" s="5" t="str">
+      <c r="AK57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:10796, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6240'. GNIS Entry Created: 6/27/1984, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>10946</v>
       </c>
@@ -8452,21 +8645,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Santa Maria Spring</v>
       </c>
-      <c r="AH58" s="2" t="s">
+      <c r="AH58" s="2"/>
+      <c r="AI58" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI58" s="3">
+      <c r="AJ58" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ58" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK58" s="5" t="str">
+      <c r="AK58" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL58" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Spring","Notes":"GNIS Feature ID:10946, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5020'. GNIS Entry Created: 2/8/1980, Updated: 4/18/2011. "}</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>11122</v>
       </c>
@@ -8563,21 +8757,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Sevenmile Tank</v>
       </c>
-      <c r="AH59" s="2" t="s">
+      <c r="AH59" s="2"/>
+      <c r="AI59" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI59" s="3">
+      <c r="AJ59" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ59" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK59" s="5" t="str">
+      <c r="AK59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL59" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:11122, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6375'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>11198</v>
       </c>
@@ -8674,21 +8869,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Sheep Tank</v>
       </c>
-      <c r="AH60" s="2" t="s">
+      <c r="AH60" s="2"/>
+      <c r="AI60" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI60" s="3">
+      <c r="AJ60" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ60" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK60" s="5" t="str">
+      <c r="AK60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL60" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:11198, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6240'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="61" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>12281</v>
       </c>
@@ -8783,21 +8979,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, The Alligator</v>
       </c>
-      <c r="AH61" s="2" t="s">
+      <c r="AH61" s="2"/>
+      <c r="AI61" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI61" s="3">
+      <c r="AJ61" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ61" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK61" s="5" t="str">
+      <c r="AK61" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL61" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:12281, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5774'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>12286</v>
       </c>
@@ -8894,21 +9091,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, The Battleship</v>
       </c>
-      <c r="AH62" s="2" t="s">
+      <c r="AH62" s="2"/>
+      <c r="AI62" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI62" s="3">
+      <c r="AJ62" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ62" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK62" s="5" t="str">
+      <c r="AK62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL62" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:12286, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5850'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>12337</v>
       </c>
@@ -9005,21 +9203,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, The Inferno</v>
       </c>
-      <c r="AH63" s="2" t="s">
+      <c r="AH63" s="2"/>
+      <c r="AI63" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI63" s="3">
+      <c r="AJ63" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ63" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK63" s="5" t="str">
+      <c r="AK63" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL63" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Ridge","Notes":"GNIS Feature ID:12337, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4163'. GNIS Entry Created: 2/8/1980, Updated: 3/22/2011. "}</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>12449</v>
       </c>
@@ -9116,21 +9315,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Thurston Tank</v>
       </c>
-      <c r="AH64" s="2" t="s">
+      <c r="AH64" s="2"/>
+      <c r="AI64" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI64" s="3">
+      <c r="AJ64" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ64" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK64" s="5" t="str">
+      <c r="AK64" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL64" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:12449, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6053'. GNIS Entry Created: 2/8/1980, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>12625</v>
       </c>
@@ -9235,21 +9435,22 @@
         <f t="shared" si="14"/>
         <v>grand canyon, Topaz Canyon</v>
       </c>
-      <c r="AH65" s="2" t="s">
+      <c r="AH65" s="2"/>
+      <c r="AI65" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI65" s="3">
+      <c r="AJ65" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ65" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK65" s="5" t="str">
+      <c r="AK65" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL65" s="5" t="str">
         <f t="shared" si="7"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Valley","Notes":"GNIS Feature ID:12625, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2654'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>12656</v>
       </c>
@@ -9346,21 +9547,22 @@
         <f t="shared" ref="AG66:AG99" si="21">_xlfn.CONCAT("grand canyon, ", B66)</f>
         <v>grand canyon, Tower of Set</v>
       </c>
-      <c r="AH66" s="2" t="s">
+      <c r="AH66" s="2"/>
+      <c r="AI66" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI66" s="3">
+      <c r="AJ66" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ66" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK66" s="5" t="str">
-        <f t="shared" ref="AK66:AK99" si="22">_xlfn.CONCAT("ContentId:||Type:Feature||Data:{""DataTypeIdentifier"":""Feature"",""Type"":""",C66,""",""Notes"":""GNIS Feature ID:",A66,", ", F66," County, ",D66,". USGS 7.5' Quad: ",R66,". GNIS Elevation: ", Q66,"'. GNIS Entry Created: ", TEXT(S66,"M/D/YYYY"),IF(ISBLANK(T66),".",_xlfn.CONCAT(", Updated: ", TEXT(T66,"M/D/YYYY"),". ")),"""}")</f>
+      <c r="AK66" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL66" s="5" t="str">
+        <f t="shared" ref="AL66:AL99" si="22">_xlfn.CONCAT("ContentId:||Type:Feature||Data:{""DataTypeIdentifier"":""Feature"",""Type"":""",C66,""",""Notes"":""GNIS Feature ID:",A66,", ", F66," County, ",D66,". USGS 7.5' Quad: ",R66,". GNIS Elevation: ", Q66,"'. GNIS Entry Created: ", TEXT(S66,"M/D/YYYY"),IF(ISBLANK(T66),".",_xlfn.CONCAT(", Updated: ", TEXT(T66,"M/D/YYYY"),". ")),"""}")</f>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:12656, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6010'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>12692</v>
       </c>
@@ -9465,21 +9667,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Travertine Canyon</v>
       </c>
-      <c r="AH67" s="2" t="s">
+      <c r="AH67" s="2"/>
+      <c r="AI67" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI67" s="3">
+      <c r="AJ67" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ67" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK67" s="5" t="str">
+      <c r="AK67" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL67" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Valley","Notes":"GNIS Feature ID:12692, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2342'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>12719</v>
       </c>
@@ -9582,21 +9785,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Trinity Creek</v>
       </c>
-      <c r="AH68" s="2" t="s">
+      <c r="AH68" s="2"/>
+      <c r="AI68" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI68" s="3">
+      <c r="AJ68" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ68" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK68" s="5" t="str">
+      <c r="AK68" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL68" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Stream","Notes":"GNIS Feature ID:12719, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 2379'. GNIS Entry Created: 2/8/1980."}</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>13220</v>
       </c>
@@ -9693,21 +9897,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Vesta Temple</v>
       </c>
-      <c r="AH69" s="2" t="s">
+      <c r="AH69" s="2"/>
+      <c r="AI69" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI69" s="3">
+      <c r="AJ69" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ69" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK69" s="5" t="str">
+      <c r="AK69" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL69" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:13220, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6302'. GNIS Entry Created: 2/8/1980, Updated: 5/16/2017. "}</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>13706</v>
       </c>
@@ -9804,21 +10009,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Whites Butte</v>
       </c>
-      <c r="AH70" s="2" t="s">
+      <c r="AH70" s="2"/>
+      <c r="AI70" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI70" s="3">
+      <c r="AJ70" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ70" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK70" s="5" t="str">
+      <c r="AK70" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL70" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Summit","Notes":"GNIS Feature ID:13706, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 4833'. GNIS Entry Created: 2/8/1980, Updated: 8/31/2018. "}</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>20722</v>
       </c>
@@ -9913,21 +10119,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Coconino Siding</v>
       </c>
-      <c r="AH71" s="2" t="s">
+      <c r="AH71" s="2"/>
+      <c r="AI71" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI71" s="3">
+      <c r="AJ71" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ71" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK71" s="5" t="str">
+      <c r="AK71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL71" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Locale","Notes":"GNIS Feature ID:20722, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6437'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>20780</v>
       </c>
@@ -10024,21 +10231,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Grand Canyon Elementary School</v>
       </c>
-      <c r="AH72" s="2" t="s">
+      <c r="AH72" s="2"/>
+      <c r="AI72" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI72" s="3">
+      <c r="AJ72" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ72" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK72" s="5" t="str">
+      <c r="AK72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL72" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"School","Notes":"GNIS Feature ID:20780, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6922'. GNIS Entry Created: 6/27/1984, Updated: 1/11/2017. "}</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>20781</v>
       </c>
@@ -10135,21 +10343,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Grand Canyon High School</v>
       </c>
-      <c r="AH73" s="2" t="s">
+      <c r="AH73" s="2"/>
+      <c r="AI73" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI73" s="3">
+      <c r="AJ73" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ73" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK73" s="5" t="str">
+      <c r="AK73" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL73" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"School","Notes":"GNIS Feature ID:20781, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6919'. GNIS Entry Created: 6/27/1984, Updated: 1/11/2017. "}</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>20782</v>
       </c>
@@ -10246,21 +10455,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, North Country Community Health Center Grand Canyon Clinic</v>
       </c>
-      <c r="AH74" s="2" t="s">
+      <c r="AH74" s="2"/>
+      <c r="AI74" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI74" s="3">
+      <c r="AJ74" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ74" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK74" s="5" t="str">
+      <c r="AK74" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL74" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Hospital","Notes":"GNIS Feature ID:20782, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6972'. GNIS Entry Created: 6/27/1984, Updated: 10/25/2018. "}</v>
       </c>
     </row>
-    <row r="75" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>20785</v>
       </c>
@@ -10357,21 +10567,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Grand Canyon Railroad Station</v>
       </c>
-      <c r="AH75" s="2" t="s">
+      <c r="AH75" s="2"/>
+      <c r="AI75" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI75" s="3">
+      <c r="AJ75" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ75" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK75" s="5" t="str">
+      <c r="AK75" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL75" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Locale","Notes":"GNIS Feature ID:20785, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6883'. GNIS Entry Created: 6/27/1984, Updated: 2/26/2010. "}</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>20798</v>
       </c>
@@ -10466,21 +10677,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Hermit Basin</v>
       </c>
-      <c r="AH76" s="2" t="s">
+      <c r="AH76" s="2"/>
+      <c r="AI76" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI76" s="3">
+      <c r="AJ76" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ76" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK76" s="5" t="str">
+      <c r="AK76" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL76" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Basin","Notes":"GNIS Feature ID:20798, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5371'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>20918</v>
       </c>
@@ -10575,21 +10787,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, National Park Service Training Center</v>
       </c>
-      <c r="AH77" s="2" t="s">
+      <c r="AH77" s="2"/>
+      <c r="AI77" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI77" s="3">
+      <c r="AJ77" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ77" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK77" s="5" t="str">
+      <c r="AK77" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL77" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"School","Notes":"GNIS Feature ID:20918, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6952'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="78" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>20988</v>
       </c>
@@ -10686,21 +10899,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Road Tank</v>
       </c>
-      <c r="AH78" s="2" t="s">
+      <c r="AH78" s="2"/>
+      <c r="AI78" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI78" s="3">
+      <c r="AJ78" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ78" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK78" s="5" t="str">
+      <c r="AK78" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL78" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:20988, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6352'. GNIS Entry Created: 6/27/1984, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="79" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>20997</v>
       </c>
@@ -10795,21 +11009,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Rowe Well Picnic Area</v>
       </c>
-      <c r="AH79" s="2" t="s">
+      <c r="AH79" s="2"/>
+      <c r="AI79" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI79" s="3">
+      <c r="AJ79" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ79" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK79" s="5" t="str">
+      <c r="AK79" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL79" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Park","Notes":"GNIS Feature ID:20997, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6594'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>20998</v>
       </c>
@@ -10904,21 +11119,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Rowes Tank</v>
       </c>
-      <c r="AH80" s="2" t="s">
+      <c r="AH80" s="2"/>
+      <c r="AI80" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI80" s="3">
+      <c r="AJ80" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ80" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK80" s="5" t="str">
+      <c r="AK80" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL80" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:20998, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6653'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="81" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>21006</v>
       </c>
@@ -11015,21 +11231,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Sewer Number One Tank</v>
       </c>
-      <c r="AH81" s="2" t="s">
+      <c r="AH81" s="2"/>
+      <c r="AI81" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI81" s="3">
+      <c r="AJ81" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ81" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK81" s="5" t="str">
+      <c r="AK81" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL81" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:21006, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6575'. GNIS Entry Created: 6/27/1984, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="82" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>21007</v>
       </c>
@@ -11126,21 +11343,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Sewer Number Two Tank</v>
       </c>
-      <c r="AH82" s="2" t="s">
+      <c r="AH82" s="2"/>
+      <c r="AI82" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI82" s="3">
+      <c r="AJ82" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ82" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK82" s="5" t="str">
+      <c r="AK82" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:21007, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6598'. GNIS Entry Created: 6/27/1984, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="83" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>21063</v>
       </c>
@@ -11235,21 +11453,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, The Abyss</v>
       </c>
-      <c r="AH83" s="2" t="s">
+      <c r="AH83" s="2"/>
+      <c r="AI83" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI83" s="3">
+      <c r="AJ83" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ83" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK83" s="5" t="str">
+      <c r="AK83" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cliff","Notes":"GNIS Feature ID:21063, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5121'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="84" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>21097</v>
       </c>
@@ -11346,21 +11565,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Upper Wagner Tank</v>
       </c>
-      <c r="AH84" s="2" t="s">
+      <c r="AH84" s="2"/>
+      <c r="AI84" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI84" s="3">
+      <c r="AJ84" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ84" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK84" s="5" t="str">
+      <c r="AK84" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL84" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:21097, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6125'. GNIS Entry Created: 6/27/1984, Updated: 3/16/2019. "}</v>
       </c>
     </row>
-    <row r="85" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>23951</v>
       </c>
@@ -11455,21 +11675,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Boucher Trail</v>
       </c>
-      <c r="AH85" s="2" t="s">
+      <c r="AH85" s="2"/>
+      <c r="AI85" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI85" s="3">
+      <c r="AJ85" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ85" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK85" s="5" t="str">
+      <c r="AK85" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL85" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Trail","Notes":"GNIS Feature ID:23951, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5915'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="86" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>24071</v>
       </c>
@@ -11564,21 +11785,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Lost Orphan Mine</v>
       </c>
-      <c r="AH86" s="2" t="s">
+      <c r="AH86" s="2"/>
+      <c r="AI86" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI86" s="3">
+      <c r="AJ86" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ86" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK86" s="5" t="str">
+      <c r="AK86" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL86" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Mine","Notes":"GNIS Feature ID:24071, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6988'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="87" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>38120</v>
       </c>
@@ -11673,21 +11895,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Trap Tank</v>
       </c>
-      <c r="AH87" s="2" t="s">
+      <c r="AH87" s="2"/>
+      <c r="AI87" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI87" s="3">
+      <c r="AJ87" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ87" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK87" s="5" t="str">
+      <c r="AK87" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL87" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Reservoir","Notes":"GNIS Feature ID:38120, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 3327'. GNIS Entry Created: 6/27/1984."}</v>
       </c>
     </row>
-    <row r="88" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>43179</v>
       </c>
@@ -11784,21 +12007,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, El Tovar Hotel</v>
       </c>
-      <c r="AH88" s="2" t="s">
+      <c r="AH88" s="2"/>
+      <c r="AI88" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI88" s="3">
+      <c r="AJ88" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ88" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK88" s="5" t="str">
+      <c r="AK88" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL88" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Building","Notes":"GNIS Feature ID:43179, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6906'. GNIS Entry Created: 2/8/1980, Updated: 11/29/2008. "}</v>
       </c>
     </row>
-    <row r="89" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>45549</v>
       </c>
@@ -11894,21 +12118,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, The Ranch Airport (historical)</v>
       </c>
-      <c r="AH89" s="2" t="s">
+      <c r="AH89" s="2"/>
+      <c r="AI89" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI89" s="3">
+      <c r="AJ89" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ89" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK89" s="5" t="str">
+      <c r="AK89" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL89" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Airport","Notes":"GNIS Feature ID:45549, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6197'. GNIS Entry Created: 8/1/1994, Updated: 8/25/2014. "}</v>
       </c>
     </row>
-    <row r="90" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>2091556</v>
       </c>
@@ -12003,21 +12228,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Waldron Trail</v>
       </c>
-      <c r="AH90" s="2" t="s">
+      <c r="AH90" s="2"/>
+      <c r="AI90" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI90" s="3">
+      <c r="AJ90" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ90" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK90" s="5" t="str">
+      <c r="AK90" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL90" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Trail","Notes":"GNIS Feature ID:2091556, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 5505'. GNIS Entry Created: 8/7/2006."}</v>
       </c>
     </row>
-    <row r="91" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>2091557</v>
       </c>
@@ -12112,21 +12338,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, West Rim Trail</v>
       </c>
-      <c r="AH91" s="2" t="s">
+      <c r="AH91" s="2"/>
+      <c r="AI91" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI91" s="3">
+      <c r="AJ91" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ91" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK91" s="5" t="str">
+      <c r="AK91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL91" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Trail","Notes":"GNIS Feature ID:2091557, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6722'. GNIS Entry Created: 8/7/2006."}</v>
       </c>
     </row>
-    <row r="92" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>2408314</v>
       </c>
@@ -12223,21 +12450,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Grand Canyon Village Census Designated Place</v>
       </c>
-      <c r="AH92" s="2" t="s">
+      <c r="AH92" s="2"/>
+      <c r="AI92" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI92" s="3">
+      <c r="AJ92" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ92" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK92" s="5" t="str">
+      <c r="AK92" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL92" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Census","Notes":"GNIS Feature ID:2408314, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6804'. GNIS Entry Created: 3/11/2008, Updated: 5/21/2020. "}</v>
       </c>
     </row>
-    <row r="93" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>2499897</v>
       </c>
@@ -12332,21 +12560,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Hopi House</v>
       </c>
-      <c r="AH93" s="2" t="s">
+      <c r="AH93" s="2"/>
+      <c r="AI93" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI93" s="3">
+      <c r="AJ93" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ93" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK93" s="5" t="str">
+      <c r="AK93" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL93" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Building","Notes":"GNIS Feature ID:2499897, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6919'. GNIS Entry Created: 11/29/2008."}</v>
       </c>
     </row>
-    <row r="94" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>2499898</v>
       </c>
@@ -12441,21 +12670,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Mary Jane Colter Lookout Studio</v>
       </c>
-      <c r="AH94" s="2" t="s">
+      <c r="AH94" s="2"/>
+      <c r="AI94" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI94" s="3">
+      <c r="AJ94" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ94" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK94" s="5" t="str">
+      <c r="AK94" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL94" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Building","Notes":"GNIS Feature ID:2499898, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6791'. GNIS Entry Created: 11/29/2008."}</v>
       </c>
     </row>
-    <row r="95" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>2500220</v>
       </c>
@@ -12550,21 +12780,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Bright Angel Lodge</v>
       </c>
-      <c r="AH95" s="2" t="s">
+      <c r="AH95" s="2"/>
+      <c r="AI95" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI95" s="3">
+      <c r="AJ95" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ95" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK95" s="5" t="str">
+      <c r="AK95" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL95" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Building","Notes":"GNIS Feature ID:2500220, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6850'. GNIS Entry Created: 11/29/2008."}</v>
       </c>
     </row>
-    <row r="96" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>2581885</v>
       </c>
@@ -12659,21 +12890,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Jicarilla Bridge</v>
       </c>
-      <c r="AH96" s="2" t="s">
+      <c r="AH96" s="2"/>
+      <c r="AI96" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI96" s="3">
+      <c r="AJ96" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ96" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK96" s="5" t="str">
+      <c r="AK96" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL96" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Arch","Notes":"GNIS Feature ID:2581885, Coconino County, AZ. USGS 7.5' Quad: Piute Point. GNIS Elevation: 6473'. GNIS Entry Created: 3/29/2010."}</v>
       </c>
     </row>
-    <row r="97" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>2669382</v>
       </c>
@@ -12770,21 +13002,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, National Park Service Grand Canyon South Rim Wastewater Treatment Facility</v>
       </c>
-      <c r="AH97" s="2" t="s">
+      <c r="AH97" s="2"/>
+      <c r="AI97" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI97" s="3">
+      <c r="AJ97" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ97" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK97" s="5" t="str">
+      <c r="AK97" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL97" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Locale","Notes":"GNIS Feature ID:2669382, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6690'. GNIS Entry Created: 7/6/2011, Updated: 10/25/2018. "}</v>
       </c>
     </row>
-    <row r="98" spans="1:37" ht="58" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>2670881</v>
       </c>
@@ -12881,21 +13114,22 @@
         <f t="shared" si="21"/>
         <v>grand canyon, El Cristo Rey Catholic Church</v>
       </c>
-      <c r="AH98" s="2" t="s">
+      <c r="AH98" s="2"/>
+      <c r="AI98" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI98" s="3">
+      <c r="AJ98" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ98" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK98" s="5" t="str">
+      <c r="AK98" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL98" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Church","Notes":"GNIS Feature ID:2670881, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6919'. GNIS Entry Created: 7/13/2011, Updated: 10/25/2018. "}</v>
       </c>
     </row>
-    <row r="99" spans="1:37" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>2789376</v>
       </c>
@@ -12990,16 +13224,17 @@
         <f t="shared" si="21"/>
         <v>grand canyon, Grand Canyon Pioneer Cemetery</v>
       </c>
-      <c r="AH99" s="2" t="s">
+      <c r="AH99" s="2"/>
+      <c r="AI99" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AI99" s="3">
+      <c r="AJ99" s="3">
         <v>44095</v>
       </c>
-      <c r="AJ99" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK99" s="5" t="str">
+      <c r="AK99" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL99" s="5" t="str">
         <f t="shared" si="22"/>
         <v>ContentId:||Type:Feature||Data:{"DataTypeIdentifier":"Feature","Type":"Cemetery","Notes":"GNIS Feature ID:2789376, Coconino County, AZ. USGS 7.5' Quad: Grand Canyon. GNIS Elevation: 6932'. GNIS Entry Created: 5/24/2018."}</v>
       </c>

</xml_diff>

<commit_message>
Improvements and Bug Fixes for Point Map, Integrate Point Labels
TextMarkerText is renamed to MapLabel and the feature is built out to include better map presentation.
Points had an error with the link protocol being doubled - fixed.
Single Lines didn't have a name pop up - fixed by added a property to the generated GeoJson.
SinglePointDiv had an error - the text caption for the map wasn't rendered correctly.
</commit_message>
<xml_diff>
--- a/PointlessWaymarks.CmsTests/TestMedia/GrandCanyonPointsImport.xlsx
+++ b/PointlessWaymarks.CmsTests/TestMedia/GrandCanyonPointsImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PointlessWaymarksCms03\PointlessWaymarks.CmsTests\TestMedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7697D7-3BFB-4F5B-853D-60629C01BB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2B6EF7-16F1-4BD0-B6C1-83A816D4B7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{A502E4A2-19B3-43B1-97B2-6120C4E9A4F5}"/>
   </bookViews>
@@ -1146,9 +1146,6 @@
     <t>PointDetail 1</t>
   </si>
   <si>
-    <t>TextMarkerText</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -1180,6 +1177,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>MapLabel</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1707,7 @@
     <tableColumn id="33" xr3:uid="{83B88F62-B46F-4CED-A530-3B101E8CBBFA}" name="Tags" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.CONCAT("grand canyon, ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{8ECFFA9E-BE30-4C9B-81AD-E8FBE61FCB97}" name="TextMarkerText" dataDxfId="4"/>
+    <tableColumn id="38" xr3:uid="{8ECFFA9E-BE30-4C9B-81AD-E8FBE61FCB97}" name="MapLabel" dataDxfId="4"/>
     <tableColumn id="34" xr3:uid="{6B0E8F35-25DB-4BD6-93F3-2E2E8DBACA78}" name="CreatedBy" dataDxfId="3"/>
     <tableColumn id="35" xr3:uid="{2CCAFA83-E69E-4E91-92D8-DF4C6DC8F9FC}" name="CreatedOn" dataDxfId="2"/>
     <tableColumn id="36" xr3:uid="{DEE1C7CE-9A12-46E0-B3F8-8B00D65FFA10}" name="UpdateContentFormat" dataDxfId="1"/>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5FEDEF-5A8E-421A-8857-D6C400357593}">
   <dimension ref="A1:AL99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X40" workbookViewId="0">
-      <selection activeCell="AH43" sqref="AH43"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,7 +2162,7 @@
         <v>329</v>
       </c>
       <c r="AH1" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="AI1" t="s">
         <v>364</v>
@@ -2275,7 +2275,7 @@
         <v>grand canyon, Bass Tank</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>362</v>
@@ -2395,7 +2395,7 @@
         <v>grand canyon, Boucher Creek</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AI3" s="2" t="s">
         <v>362</v>
@@ -2509,7 +2509,7 @@
         <v>grand canyon, Boucher Rapids</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AI4" s="2" t="s">
         <v>362</v>
@@ -2621,7 +2621,7 @@
         <v>grand canyon, Breezy Point</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AI5" s="2" t="s">
         <v>362</v>
@@ -2735,7 +2735,7 @@
         <v>grand canyon, Bright Angel Trail</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AI6" s="2" t="s">
         <v>362</v>
@@ -2855,7 +2855,7 @@
         <v>grand canyon, Bright Angel Wash</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AI7" s="2" t="s">
         <v>362</v>
@@ -2969,7 +2969,7 @@
         <v>grand canyon, Brush Tank</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AI8" s="2" t="s">
         <v>362</v>
@@ -3081,7 +3081,7 @@
         <v>grand canyon, Cathedral Stairs</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AI9" s="2" t="s">
         <v>362</v>
@@ -3195,7 +3195,7 @@
         <v>grand canyon, Cedar Spring</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AI10" s="2" t="s">
         <v>362</v>
@@ -3307,7 +3307,7 @@
         <v>grand canyon, Cocopa Point</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AI11" s="2" t="s">
         <v>362</v>
@@ -3419,7 +3419,7 @@
         <v>grand canyon, Columbus Point</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AI12" s="2" t="s">
         <v>362</v>
@@ -3533,7 +3533,7 @@
         <v>grand canyon, Cope Butte</v>
       </c>
       <c r="AH13" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AI13" s="2" t="s">
         <v>362</v>
@@ -3647,7 +3647,7 @@
         <v>grand canyon, Dana Butte</v>
       </c>
       <c r="AH14" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AI14" s="2" t="s">
         <v>362</v>
@@ -3761,7 +3761,7 @@
         <v>grand canyon, Diana Temple</v>
       </c>
       <c r="AH15" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AI15" s="2" t="s">
         <v>362</v>
@@ -3875,7 +3875,7 @@
         <v>grand canyon, Dripping Spring</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AI16" s="2" t="s">
         <v>362</v>
@@ -3987,7 +3987,7 @@
         <v>grand canyon, Dripping Springs Trail</v>
       </c>
       <c r="AH17" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AI17" s="2" t="s">
         <v>362</v>
@@ -4101,7 +4101,7 @@
         <v>grand canyon, Eremita Mesa</v>
       </c>
       <c r="AH18" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AI18" s="2" t="s">
         <v>362</v>
@@ -4215,7 +4215,7 @@
         <v>grand canyon, Eremita Tank</v>
       </c>
       <c r="AH19" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AI19" s="2" t="s">
         <v>362</v>
@@ -4327,7 +4327,7 @@
         <v>grand canyon, Fourmile Spring</v>
       </c>
       <c r="AH20" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AI20" s="2" t="s">
         <v>362</v>
@@ -4441,7 +4441,7 @@
         <v>grand canyon, Grand Canyon</v>
       </c>
       <c r="AH21" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AI21" s="2" t="s">
         <v>362</v>
@@ -4555,7 +4555,7 @@
         <v>grand canyon, Granite Rapids</v>
       </c>
       <c r="AH22" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AI22" s="2" t="s">
         <v>362</v>
@@ -4667,7 +4667,7 @@
         <v>grand canyon, Great Mohave Wall</v>
       </c>
       <c r="AH23" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AI23" s="2" t="s">
         <v>362</v>
@@ -4787,7 +4787,7 @@
         <v>grand canyon, Hermit Creek</v>
       </c>
       <c r="AH24" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI24" s="2" t="s">
         <v>362</v>
@@ -4901,7 +4901,7 @@
         <v>grand canyon, Hermit Rapids</v>
       </c>
       <c r="AH25" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI25" s="2" t="s">
         <v>362</v>
@@ -5013,7 +5013,7 @@
         <v>grand canyon, Hermit Trail</v>
       </c>
       <c r="AH26" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI26" s="2" t="s">
         <v>362</v>
@@ -5125,7 +5125,7 @@
         <v>grand canyon, Hermits Rest</v>
       </c>
       <c r="AH27" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI27" s="2" t="s">
         <v>362</v>
@@ -5239,7 +5239,7 @@
         <v>grand canyon, Homestead Tank</v>
       </c>
       <c r="AH28" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI28" s="2" t="s">
         <v>362</v>
@@ -5351,7 +5351,7 @@
         <v>grand canyon, Hopi Point</v>
       </c>
       <c r="AH29" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI29" s="2" t="s">
         <v>362</v>
@@ -5465,7 +5465,7 @@
         <v>grand canyon, Hopi Wall</v>
       </c>
       <c r="AH30" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI30" s="2" t="s">
         <v>362</v>
@@ -5585,7 +5585,7 @@
         <v>grand canyon, Horn Creek</v>
       </c>
       <c r="AH31" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI31" s="2" t="s">
         <v>362</v>
@@ -5699,7 +5699,7 @@
         <v>grand canyon, Horn Creek Rapids</v>
       </c>
       <c r="AH32" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI32" s="2" t="s">
         <v>362</v>
@@ -5813,7 +5813,7 @@
         <v>grand canyon, Horsethief Tank</v>
       </c>
       <c r="AH33" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AI33" s="2" t="s">
         <v>362</v>
@@ -5927,7 +5927,7 @@
         <v>grand canyon, Ike Smith Tank</v>
       </c>
       <c r="AH34" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AI34" s="2" t="s">
         <v>362</v>
@@ -6039,7 +6039,7 @@
         <v>grand canyon, Jicarilla Point</v>
       </c>
       <c r="AH35" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AI35" s="2" t="s">
         <v>362</v>
@@ -6153,7 +6153,7 @@
         <v>grand canyon, Little Rain Tank</v>
       </c>
       <c r="AH36" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AI36" s="2" t="s">
         <v>362</v>
@@ -6265,7 +6265,7 @@
         <v>grand canyon, Lookout Point</v>
       </c>
       <c r="AH37" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AI37" s="2" t="s">
         <v>362</v>
@@ -6377,7 +6377,7 @@
         <v>grand canyon, Maricopa Point</v>
       </c>
       <c r="AH38" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI38" s="2" t="s">
         <v>362</v>
@@ -6491,7 +6491,7 @@
         <v>grand canyon, Marsh Butte</v>
       </c>
       <c r="AH39" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI39" s="2" t="s">
         <v>362</v>
@@ -6603,7 +6603,7 @@
         <v>grand canyon, Mescalero Point</v>
       </c>
       <c r="AH40" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI40" s="2" t="s">
         <v>362</v>
@@ -6717,7 +6717,7 @@
         <v>grand canyon, Midway Number One Tank</v>
       </c>
       <c r="AH41" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI41" s="2" t="s">
         <v>362</v>
@@ -6831,7 +6831,7 @@
         <v>grand canyon, Midway Number Two Tank</v>
       </c>
       <c r="AH42" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI42" s="2" t="s">
         <v>362</v>
@@ -6943,7 +6943,7 @@
         <v>grand canyon, Mimbreno Point</v>
       </c>
       <c r="AH43" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI43" s="2" t="s">
         <v>362</v>
@@ -7055,7 +7055,7 @@
         <v>grand canyon, Mohave Point</v>
       </c>
       <c r="AH44" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI44" s="2" t="s">
         <v>362</v>
@@ -7175,7 +7175,7 @@
         <v>grand canyon, Monument Creek</v>
       </c>
       <c r="AH45" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AI45" s="2" t="s">
         <v>362</v>

</xml_diff>